<commit_message>
open xml file button
</commit_message>
<xml_diff>
--- a/src/ptm2 scheduler.xlsx
+++ b/src/ptm2 scheduler.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kfirb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kfirb\IdeaProjects\ptm2\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F887F17-FC6D-4E33-938B-55661BC70519}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDFE4D1-88DF-4EC0-B45A-8C754512300D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1383,6 +1383,66 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1399,66 +1459,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="35" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="35" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="35" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1818,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1835,16 +1835,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
@@ -1885,16 +1885,16 @@
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="26" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1911,10 +1911,10 @@
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="38"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
@@ -1929,10 +1929,10 @@
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="38"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
@@ -1947,10 +1947,10 @@
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="38"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
@@ -1965,14 +1965,14 @@
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="38"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
@@ -1987,10 +1987,10 @@
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="38"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="27"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
@@ -2005,10 +2005,10 @@
       <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="38"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="27"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
@@ -2023,10 +2023,10 @@
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="38"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
@@ -2041,14 +2041,14 @@
       <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="38"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
@@ -2063,10 +2063,10 @@
       <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="38"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
@@ -2081,28 +2081,28 @@
       <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="38"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="27"/>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="43"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
@@ -2117,16 +2117,16 @@
       <c r="D15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="34">
+      <c r="H15" s="29">
         <v>4</v>
       </c>
     </row>
@@ -2143,10 +2143,10 @@
       <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="35"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
@@ -2161,10 +2161,10 @@
       <c r="D17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="35"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="30"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
@@ -2179,10 +2179,10 @@
       <c r="D18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="35"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="30"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
@@ -2197,10 +2197,10 @@
       <c r="D19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="35"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="30"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
@@ -2215,14 +2215,14 @@
       <c r="D20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="35"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="30"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
@@ -2237,10 +2237,10 @@
       <c r="D21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="35"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -2255,10 +2255,10 @@
       <c r="D22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="35"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="30"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
@@ -2273,28 +2273,28 @@
       <c r="D23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="35"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="30"/>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="36"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="31"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
@@ -2309,16 +2309,16 @@
       <c r="D25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="H25" s="34">
+      <c r="H25" s="29">
         <v>5</v>
       </c>
     </row>
@@ -2335,10 +2335,10 @@
       <c r="D26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="35"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="30"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
@@ -2353,10 +2353,10 @@
       <c r="D27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="35"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="30"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
@@ -2371,10 +2371,10 @@
       <c r="D28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="35"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="30"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
@@ -2389,10 +2389,10 @@
       <c r="D29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="35"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="30"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
@@ -2407,10 +2407,10 @@
       <c r="D30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="35"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="30"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
@@ -2425,10 +2425,10 @@
       <c r="D31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="27"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="35"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="30"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
@@ -2443,10 +2443,10 @@
       <c r="D32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="27"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="35"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="30"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
@@ -2461,10 +2461,10 @@
       <c r="D33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="35"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="30"/>
     </row>
     <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="11" t="s">
@@ -2479,10 +2479,10 @@
       <c r="D34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="36"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="31"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
@@ -2497,16 +2497,16 @@
       <c r="D35" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="32" t="s">
+      <c r="E35" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="F35" s="29" t="s">
+      <c r="F35" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="29" t="s">
+      <c r="G35" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="H35" s="34">
+      <c r="H35" s="29">
         <v>6</v>
       </c>
     </row>
@@ -2523,10 +2523,10 @@
       <c r="D36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="35"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="30"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2541,10 +2541,10 @@
       <c r="D37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="35"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="30"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
@@ -2559,10 +2559,10 @@
       <c r="D38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="35"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="30"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2577,10 +2577,10 @@
       <c r="D39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E39" s="27"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="35"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="30"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
@@ -2595,10 +2595,10 @@
       <c r="D40" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E40" s="27"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="35"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="30"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
@@ -2613,10 +2613,10 @@
       <c r="D41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="35"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="30"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
@@ -2631,10 +2631,10 @@
       <c r="D42" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E42" s="27"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="35"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="30"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
@@ -2649,10 +2649,10 @@
       <c r="D43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="35"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="30"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
@@ -2667,10 +2667,10 @@
       <c r="D44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="35"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="30"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
@@ -2685,10 +2685,10 @@
       <c r="D45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E45" s="27"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="35"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="30"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
@@ -2703,14 +2703,14 @@
       <c r="D46" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E46" s="27" t="s">
+      <c r="E46" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="F46" s="31" t="s">
+      <c r="F46" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="G46" s="31"/>
-      <c r="H46" s="35"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="30"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
@@ -2725,10 +2725,10 @@
       <c r="D47" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="27"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="35"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="30"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
@@ -2743,10 +2743,10 @@
       <c r="D48" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E48" s="27"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="35"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="30"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
@@ -2761,10 +2761,10 @@
       <c r="D49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="27"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="35"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="30"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
@@ -2779,10 +2779,10 @@
       <c r="D50" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E50" s="27"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="35"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="30"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
@@ -2797,10 +2797,10 @@
       <c r="D51" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="27"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="35"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="30"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
@@ -2815,10 +2815,10 @@
       <c r="D52" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E52" s="27"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="35"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="30"/>
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="17" t="s">
@@ -2833,10 +2833,10 @@
       <c r="D53" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E53" s="28"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="36"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="31"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
@@ -2851,16 +2851,16 @@
       <c r="D54" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E54" s="32" t="s">
+      <c r="E54" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F54" s="29" t="s">
+      <c r="F54" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="G54" s="29" t="s">
+      <c r="G54" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="H54" s="34">
+      <c r="H54" s="29">
         <v>7</v>
       </c>
     </row>
@@ -2877,10 +2877,10 @@
       <c r="D55" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E55" s="27"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-      <c r="H55" s="35"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="30"/>
     </row>
     <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="17" t="s">
@@ -2895,10 +2895,10 @@
       <c r="D56" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E56" s="28"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="36"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="31"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="15" t="s">
@@ -2913,16 +2913,16 @@
       <c r="D57" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E57" s="32" t="s">
+      <c r="E57" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="F57" s="29" t="s">
+      <c r="F57" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="G57" s="29" t="s">
+      <c r="G57" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="H57" s="34">
+      <c r="H57" s="29">
         <v>8</v>
       </c>
     </row>
@@ -2939,10 +2939,10 @@
       <c r="D58" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E58" s="28"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="30"/>
-      <c r="H58" s="36"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="31"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
@@ -2957,16 +2957,16 @@
       <c r="D59" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E59" s="32" t="s">
+      <c r="E59" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="F59" s="29" t="s">
+      <c r="F59" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="G59" s="29" t="s">
+      <c r="G59" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="H59" s="34">
+      <c r="H59" s="29">
         <v>9</v>
       </c>
     </row>
@@ -2983,10 +2983,10 @@
       <c r="D60" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E60" s="27"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="35"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="30"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
@@ -3001,14 +3001,14 @@
       <c r="D61" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E61" s="27" t="s">
+      <c r="E61" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="F61" s="31" t="s">
+      <c r="F61" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="G61" s="31"/>
-      <c r="H61" s="35"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="30"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="13" t="s">
@@ -3023,10 +3023,10 @@
       <c r="D62" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E62" s="27"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
-      <c r="H62" s="35"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="30"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
@@ -3041,10 +3041,10 @@
       <c r="D63" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E63" s="27"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-      <c r="H63" s="35"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="30"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
@@ -3059,10 +3059,10 @@
       <c r="D64" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E64" s="27"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="31"/>
-      <c r="H64" s="35"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="30"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
@@ -3077,10 +3077,10 @@
       <c r="D65" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E65" s="27"/>
-      <c r="F65" s="31"/>
-      <c r="G65" s="31"/>
-      <c r="H65" s="35"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="30"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="13" t="s">
@@ -3095,10 +3095,10 @@
       <c r="D66" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E66" s="27"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="31"/>
-      <c r="H66" s="35"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="30"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
@@ -3113,10 +3113,10 @@
       <c r="D67" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E67" s="27"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="31"/>
-      <c r="H67" s="35"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="30"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
@@ -3131,10 +3131,10 @@
       <c r="D68" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E68" s="27"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="35"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="30"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="13" t="s">
@@ -3149,10 +3149,10 @@
       <c r="D69" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E69" s="27"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="31"/>
-      <c r="H69" s="35"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="30"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="13" t="s">
@@ -3167,14 +3167,14 @@
       <c r="D70" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E70" s="27" t="s">
+      <c r="E70" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="F70" s="31" t="s">
+      <c r="F70" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="G70" s="31"/>
-      <c r="H70" s="35"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="30"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="13" t="s">
@@ -3189,10 +3189,10 @@
       <c r="D71" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E71" s="27"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="35"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="33"/>
+      <c r="H71" s="30"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="13" t="s">
@@ -3207,10 +3207,10 @@
       <c r="D72" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E72" s="27"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="35"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="33"/>
+      <c r="G72" s="33"/>
+      <c r="H72" s="30"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="13" t="s">
@@ -3225,10 +3225,10 @@
       <c r="D73" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E73" s="27"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="35"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="33"/>
+      <c r="H73" s="30"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
@@ -3243,10 +3243,10 @@
       <c r="D74" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E74" s="27"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="35"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="33"/>
+      <c r="H74" s="30"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="13" t="s">
@@ -3261,10 +3261,10 @@
       <c r="D75" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E75" s="27"/>
-      <c r="F75" s="31"/>
-      <c r="G75" s="31"/>
-      <c r="H75" s="35"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="30"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="13" t="s">
@@ -3279,10 +3279,10 @@
       <c r="D76" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E76" s="27"/>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31"/>
-      <c r="H76" s="35"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="30"/>
     </row>
     <row r="77" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="17" t="s">
@@ -3297,10 +3297,10 @@
       <c r="D77" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E77" s="28"/>
-      <c r="F77" s="30"/>
-      <c r="G77" s="30"/>
-      <c r="H77" s="36"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="35"/>
+      <c r="H77" s="31"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
@@ -3315,16 +3315,16 @@
       <c r="D78" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E78" s="32" t="s">
+      <c r="E78" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="F78" s="29" t="s">
+      <c r="F78" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="G78" s="29" t="s">
+      <c r="G78" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="H78" s="37" t="s">
+      <c r="H78" s="26" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3341,10 +3341,10 @@
       <c r="D79" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E79" s="27"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="31"/>
-      <c r="H79" s="38"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="33"/>
+      <c r="H79" s="27"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="13" t="s">
@@ -3359,10 +3359,10 @@
       <c r="D80" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E80" s="27"/>
-      <c r="F80" s="31"/>
-      <c r="G80" s="31"/>
-      <c r="H80" s="38"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="27"/>
     </row>
     <row r="81" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="17" t="s">
@@ -3377,9 +3377,9 @@
       <c r="D81" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E81" s="28"/>
-      <c r="F81" s="30"/>
-      <c r="G81" s="30"/>
+      <c r="E81" s="38"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="35"/>
       <c r="H81" s="39"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
@@ -3395,16 +3395,16 @@
       <c r="D82" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E82" s="32" t="s">
+      <c r="E82" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="F82" s="29" t="s">
+      <c r="F82" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="G82" s="29" t="s">
+      <c r="G82" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="H82" s="34">
+      <c r="H82" s="29">
         <v>12</v>
       </c>
     </row>
@@ -3421,10 +3421,10 @@
       <c r="D83" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E83" s="28"/>
-      <c r="F83" s="30"/>
-      <c r="G83" s="30"/>
-      <c r="H83" s="36"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="35"/>
+      <c r="H83" s="31"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="19" t="s">
@@ -3439,16 +3439,16 @@
       <c r="D84" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E84" s="21" t="s">
+      <c r="E84" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="F84" s="23" t="s">
+      <c r="F84" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="G84" s="23" t="s">
+      <c r="G84" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="H84" s="25">
+      <c r="H84" s="45">
         <v>13</v>
       </c>
     </row>
@@ -3465,13 +3465,50 @@
       <c r="D85" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E85" s="22"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
-      <c r="H85" s="26"/>
+      <c r="E85" s="42"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="G84:G85"/>
+    <mergeCell ref="H84:H85"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="F70:F77"/>
+    <mergeCell ref="F61:F69"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="E70:E77"/>
+    <mergeCell ref="E61:E69"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="F54:F56"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="E46:E53"/>
+    <mergeCell ref="E35:E45"/>
+    <mergeCell ref="F46:F53"/>
+    <mergeCell ref="F35:F45"/>
+    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="G59:G77"/>
+    <mergeCell ref="G78:G81"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="H54:H56"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="H59:H77"/>
+    <mergeCell ref="H78:H81"/>
+    <mergeCell ref="H82:H83"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="H3:H14"/>
     <mergeCell ref="H15:H24"/>
@@ -3488,43 +3525,6 @@
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="F25:F34"/>
     <mergeCell ref="E25:E34"/>
-    <mergeCell ref="G78:G81"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="H54:H56"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="H59:H77"/>
-    <mergeCell ref="H78:H81"/>
-    <mergeCell ref="H82:H83"/>
-    <mergeCell ref="F46:F53"/>
-    <mergeCell ref="F35:F45"/>
-    <mergeCell ref="G54:G56"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="G59:G77"/>
-    <mergeCell ref="E15:E19"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="E46:E53"/>
-    <mergeCell ref="E35:E45"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="G84:G85"/>
-    <mergeCell ref="H84:H85"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="F70:F77"/>
-    <mergeCell ref="F61:F69"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="E70:E77"/>
-    <mergeCell ref="E61:E69"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="F54:F56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>